<commit_message>
worked on LSTM model
</commit_message>
<xml_diff>
--- a/Code/Simon/preparedData.xlsx
+++ b/Code/Simon/preparedData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonmclain/Documents/Documents/Software Development with AI/Semister 4/Engineering Team Project/TUS-Engineering-Team-Project/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonmclain/Documents/Documents/Software Development with AI/Semister 4/Engineering Team Project/TUS-Engineering-Team-Project/Code/Simon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BE767B-DD53-A948-A333-7E18B612B486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D9CD9-5970-1048-BE7E-9A4FBA2A70AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="500" windowWidth="30460" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -236,7 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX703"/>
+  <dimension ref="A1:AX700"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C682" workbookViewId="0">
+      <selection activeCell="C701" sqref="A701:XFD703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -106951,387 +106951,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="701" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A701" s="2">
-        <v>44604</v>
-      </c>
-      <c r="B701">
-        <v>5270.2860000000001</v>
-      </c>
-      <c r="C701">
-        <v>0.87</v>
-      </c>
-      <c r="D701">
-        <v>15816</v>
-      </c>
-      <c r="E701">
-        <v>0</v>
-      </c>
-      <c r="F701">
-        <v>0</v>
-      </c>
-      <c r="G701">
-        <v>10497384</v>
-      </c>
-      <c r="H701">
-        <v>4036742</v>
-      </c>
-      <c r="I701">
-        <v>3934569</v>
-      </c>
-      <c r="J701">
-        <v>2764612</v>
-      </c>
-      <c r="K701">
-        <v>12214</v>
-      </c>
-      <c r="L701">
-        <v>0</v>
-      </c>
-      <c r="M701">
-        <v>4982904</v>
-      </c>
-      <c r="N701">
-        <v>69.873999999999995</v>
-      </c>
-      <c r="O701">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="P701">
-        <v>13.928000000000001</v>
-      </c>
-      <c r="Q701">
-        <v>8.6780000000000008</v>
-      </c>
-      <c r="R701">
-        <v>67335.293000000005</v>
-      </c>
-      <c r="S701">
-        <v>0.2</v>
-      </c>
-      <c r="T701">
-        <v>126.459</v>
-      </c>
-      <c r="U701">
-        <v>3.28</v>
-      </c>
-      <c r="V701">
-        <v>23</v>
-      </c>
-      <c r="W701">
-        <v>25.7</v>
-      </c>
-      <c r="X701">
-        <v>82.3</v>
-      </c>
-      <c r="Y701">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="Z701">
-        <v>16</v>
-      </c>
-      <c r="AA701">
-        <v>3</v>
-      </c>
-      <c r="AB701">
-        <v>0</v>
-      </c>
-      <c r="AC701">
-        <v>5</v>
-      </c>
-      <c r="AD701">
-        <v>0</v>
-      </c>
-      <c r="AE701">
-        <v>3</v>
-      </c>
-      <c r="AF701">
-        <v>1</v>
-      </c>
-      <c r="AG701">
-        <v>5</v>
-      </c>
-      <c r="AH701">
-        <v>7</v>
-      </c>
-      <c r="AI701">
-        <v>3</v>
-      </c>
-      <c r="AJ701">
-        <v>4</v>
-      </c>
-      <c r="AK701">
-        <v>9</v>
-      </c>
-      <c r="AL701">
-        <v>0</v>
-      </c>
-      <c r="AM701">
-        <v>0</v>
-      </c>
-      <c r="AN701">
-        <v>3</v>
-      </c>
-      <c r="AO701">
-        <v>3</v>
-      </c>
-      <c r="AP701">
-        <v>3</v>
-      </c>
-      <c r="AQ701">
-        <v>2</v>
-      </c>
-      <c r="AR701">
-        <v>1</v>
-      </c>
-      <c r="AS701">
-        <v>0</v>
-      </c>
-      <c r="AT701">
-        <v>0</v>
-      </c>
-      <c r="AU701">
-        <v>3</v>
-      </c>
-      <c r="AV701">
-        <v>4</v>
-      </c>
-      <c r="AW701">
-        <v>0</v>
-      </c>
-      <c r="AX701">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="702" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A702" s="2">
-        <v>44605</v>
-      </c>
-      <c r="B702">
-        <v>5270.2860000000001</v>
-      </c>
-      <c r="C702">
-        <v>0</v>
-      </c>
-      <c r="D702">
-        <v>13624</v>
-      </c>
-      <c r="E702">
-        <v>0</v>
-      </c>
-      <c r="F702">
-        <v>0</v>
-      </c>
-      <c r="G702">
-        <v>10507477</v>
-      </c>
-      <c r="H702">
-        <v>4038305</v>
-      </c>
-      <c r="I702">
-        <v>3939271</v>
-      </c>
-      <c r="J702">
-        <v>2768440</v>
-      </c>
-      <c r="K702">
-        <v>10093</v>
-      </c>
-      <c r="L702">
-        <v>0</v>
-      </c>
-      <c r="M702">
-        <v>4982904</v>
-      </c>
-      <c r="N702">
-        <v>69.873999999999995</v>
-      </c>
-      <c r="O702">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="P702">
-        <v>13.928000000000001</v>
-      </c>
-      <c r="Q702">
-        <v>8.6780000000000008</v>
-      </c>
-      <c r="R702">
-        <v>67335.293000000005</v>
-      </c>
-      <c r="S702">
-        <v>0.2</v>
-      </c>
-      <c r="T702">
-        <v>126.459</v>
-      </c>
-      <c r="U702">
-        <v>3.28</v>
-      </c>
-      <c r="V702">
-        <v>23</v>
-      </c>
-      <c r="W702">
-        <v>25.7</v>
-      </c>
-      <c r="X702">
-        <v>82.3</v>
-      </c>
-      <c r="Y702">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="Z702">
-        <v>16</v>
-      </c>
-      <c r="AA702">
-        <v>3</v>
-      </c>
-      <c r="AB702">
-        <v>0</v>
-      </c>
-      <c r="AC702">
-        <v>5</v>
-      </c>
-      <c r="AD702">
-        <v>0</v>
-      </c>
-      <c r="AE702">
-        <v>3</v>
-      </c>
-      <c r="AF702">
-        <v>1</v>
-      </c>
-      <c r="AG702">
-        <v>5</v>
-      </c>
-      <c r="AH702">
-        <v>7</v>
-      </c>
-      <c r="AI702">
-        <v>3</v>
-      </c>
-      <c r="AJ702">
-        <v>4</v>
-      </c>
-      <c r="AK702">
-        <v>9</v>
-      </c>
-      <c r="AL702">
-        <v>0</v>
-      </c>
-      <c r="AM702">
-        <v>0</v>
-      </c>
-      <c r="AN702">
-        <v>3</v>
-      </c>
-      <c r="AO702">
-        <v>3</v>
-      </c>
-      <c r="AP702">
-        <v>3</v>
-      </c>
-      <c r="AQ702">
-        <v>2</v>
-      </c>
-      <c r="AR702">
-        <v>1</v>
-      </c>
-      <c r="AS702">
-        <v>0</v>
-      </c>
-      <c r="AT702">
-        <v>0</v>
-      </c>
-      <c r="AU702">
-        <v>3</v>
-      </c>
-      <c r="AV702">
-        <v>4</v>
-      </c>
-      <c r="AW702">
-        <v>0</v>
-      </c>
-      <c r="AX702">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="703" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A703" s="2">
-        <v>44606</v>
-      </c>
-      <c r="B703">
-        <v>4927</v>
-      </c>
-      <c r="C703">
-        <v>0</v>
-      </c>
-      <c r="D703">
-        <v>11943</v>
-      </c>
-      <c r="E703">
-        <v>0</v>
-      </c>
-      <c r="F703">
-        <v>0</v>
-      </c>
-      <c r="G703">
-        <v>0</v>
-      </c>
-      <c r="H703">
-        <v>0</v>
-      </c>
-      <c r="I703">
-        <v>0</v>
-      </c>
-      <c r="J703">
-        <v>0</v>
-      </c>
-      <c r="K703">
-        <v>0</v>
-      </c>
-      <c r="L703">
-        <v>0</v>
-      </c>
-      <c r="M703">
-        <v>4982904</v>
-      </c>
-      <c r="N703">
-        <v>69.873999999999995</v>
-      </c>
-      <c r="O703">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="P703">
-        <v>13.928000000000001</v>
-      </c>
-      <c r="Q703">
-        <v>8.6780000000000008</v>
-      </c>
-      <c r="R703">
-        <v>67335.293000000005</v>
-      </c>
-      <c r="S703">
-        <v>0.2</v>
-      </c>
-      <c r="T703">
-        <v>126.459</v>
-      </c>
-      <c r="U703">
-        <v>3.28</v>
-      </c>
-      <c r="V703">
-        <v>23</v>
-      </c>
-      <c r="W703">
-        <v>25.7</v>
-      </c>
-      <c r="X703">
-        <v>82.3</v>
-      </c>
-      <c r="Y703">
-        <v>0.95499999999999996</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:AX1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>